<commit_message>
Added inflow --> birth error
</commit_message>
<xml_diff>
--- a/data/validate_cascade.xlsx
+++ b/data/validate_cascade.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25035" windowHeight="14955" tabRatio="647" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" tabRatio="647" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -16,6 +21,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="638">
   <si>
     <t>Code Label</t>
   </si>
@@ -3396,13 +3404,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>75</v>
       </c>
@@ -3410,7 +3418,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
@@ -3418,7 +3426,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>547</v>
       </c>
@@ -3426,7 +3434,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>546</v>
       </c>
@@ -3434,7 +3442,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>252</v>
       </c>
@@ -3442,7 +3450,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>451</v>
       </c>
@@ -3450,7 +3458,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>431</v>
       </c>
@@ -3458,7 +3466,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>465</v>
       </c>
@@ -3466,7 +3474,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>430</v>
       </c>
@@ -3474,7 +3482,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>466</v>
       </c>
@@ -3482,7 +3490,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>448</v>
       </c>
@@ -3492,11 +3500,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3508,17 +3511,17 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3552,7 +3555,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -3574,7 +3577,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -3585,7 +3588,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -3596,7 +3599,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>186</v>
       </c>
@@ -3618,7 +3621,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -3723,7 +3726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -3734,7 +3737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -3756,7 +3759,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -3767,7 +3770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -3825,7 +3828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -3836,7 +3839,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -3847,7 +3850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -3880,7 +3883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -3891,7 +3894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3905,7 +3908,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>246</v>
       </c>
@@ -3935,11 +3938,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3947,47 +3945,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" customWidth="1"/>
-    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.33203125" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>246</v>
@@ -4092,7 +4090,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>246</v>
       </c>
@@ -4135,7 +4133,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4180,7 +4178,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4223,7 +4221,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>182</v>
       </c>
@@ -4270,7 +4268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>183</v>
       </c>
@@ -4317,7 +4315,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>184</v>
       </c>
@@ -4362,7 +4360,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>185</v>
       </c>
@@ -4407,7 +4405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>186</v>
       </c>
@@ -4452,7 +4450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>187</v>
       </c>
@@ -4497,7 +4495,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>
@@ -4540,7 +4538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>179</v>
       </c>
@@ -4583,7 +4581,7 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="22"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>180</v>
       </c>
@@ -4628,7 +4626,7 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="11"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>104</v>
       </c>
@@ -4675,7 +4673,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>105</v>
       </c>
@@ -4722,7 +4720,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>106</v>
       </c>
@@ -4771,7 +4769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>107</v>
       </c>
@@ -4818,7 +4816,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>108</v>
       </c>
@@ -4865,7 +4863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
@@ -4914,7 +4912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>110</v>
       </c>
@@ -4961,7 +4959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>111</v>
       </c>
@@ -5008,7 +5006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>112</v>
       </c>
@@ -5055,7 +5053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>181</v>
       </c>
@@ -5100,7 +5098,7 @@
       <c r="AH23" s="7"/>
       <c r="AI23" s="8"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>113</v>
       </c>
@@ -5147,7 +5145,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>114</v>
       </c>
@@ -5194,7 +5192,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>115</v>
       </c>
@@ -5243,7 +5241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>116</v>
       </c>
@@ -5290,7 +5288,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>117</v>
       </c>
@@ -5337,7 +5335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>118</v>
       </c>
@@ -5386,11 +5384,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="55" t="s">
+        <v>361</v>
+      </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -5433,7 +5433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>121</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
@@ -5570,11 +5570,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="55" t="s">
+        <v>361</v>
+      </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -5611,7 +5613,7 @@
       <c r="AH34" s="10"/>
       <c r="AI34" s="11"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
@@ -5657,11 +5659,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5673,35 +5670,35 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
-    <col min="17" max="18" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5733,7 +5730,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -5756,7 +5753,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>486</v>
       </c>
@@ -5779,7 +5776,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>470</v>
       </c>
@@ -5799,7 +5796,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>471</v>
       </c>
@@ -5822,7 +5819,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>481</v>
       </c>
@@ -5848,7 +5845,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>476</v>
       </c>
@@ -5871,7 +5868,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>475</v>
       </c>
@@ -5897,7 +5894,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>479</v>
       </c>
@@ -5923,7 +5920,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>468</v>
       </c>
@@ -5946,7 +5943,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>469</v>
       </c>
@@ -5972,7 +5969,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -5998,7 +5995,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>488</v>
       </c>
@@ -6021,7 +6018,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>517</v>
       </c>
@@ -6044,7 +6041,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>518</v>
       </c>
@@ -6067,7 +6064,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>519</v>
       </c>
@@ -6090,7 +6087,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>520</v>
       </c>
@@ -6113,7 +6110,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>522</v>
       </c>
@@ -6136,7 +6133,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>521</v>
       </c>
@@ -6159,7 +6156,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>505</v>
       </c>
@@ -6185,7 +6182,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>506</v>
       </c>
@@ -6211,7 +6208,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>507</v>
       </c>
@@ -6237,7 +6234,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>508</v>
       </c>
@@ -6263,7 +6260,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>509</v>
       </c>
@@ -6289,7 +6286,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>510</v>
       </c>
@@ -6315,7 +6312,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>493</v>
       </c>
@@ -6341,7 +6338,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>495</v>
       </c>
@@ -6367,7 +6364,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>497</v>
       </c>
@@ -6393,7 +6390,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>499</v>
       </c>
@@ -6419,7 +6416,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>500</v>
       </c>
@@ -6445,7 +6442,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>501</v>
       </c>
@@ -6471,7 +6468,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -6503,7 +6500,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>153</v>
       </c>
@@ -6535,7 +6532,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -6564,7 +6561,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -6602,7 +6599,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -6622,7 +6619,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -6642,7 +6639,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -6662,7 +6659,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>150</v>
       </c>
@@ -6682,7 +6679,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>151</v>
       </c>
@@ -6702,7 +6699,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>152</v>
       </c>
@@ -6722,7 +6719,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -6745,7 +6742,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -6768,7 +6765,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -6791,7 +6788,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -6814,7 +6811,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -6838,7 +6835,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -6861,7 +6858,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -6884,7 +6881,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>554</v>
       </c>
@@ -6907,7 +6904,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>556</v>
       </c>
@@ -6930,7 +6927,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>557</v>
       </c>
@@ -6953,7 +6950,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>560</v>
       </c>
@@ -6976,7 +6973,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>561</v>
       </c>
@@ -6999,7 +6996,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>562</v>
       </c>
@@ -7022,7 +7019,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -7045,7 +7042,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>157</v>
       </c>
@@ -7068,7 +7065,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -7091,7 +7088,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>312</v>
       </c>
@@ -7108,7 +7105,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>568</v>
       </c>
@@ -7131,7 +7128,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>571</v>
       </c>
@@ -7154,7 +7151,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>575</v>
       </c>
@@ -7177,7 +7174,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>577</v>
       </c>
@@ -7200,7 +7197,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>583</v>
       </c>
@@ -7223,7 +7220,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>585</v>
       </c>
@@ -7246,7 +7243,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>587</v>
       </c>
@@ -7269,7 +7266,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>569</v>
       </c>
@@ -7292,7 +7289,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>573</v>
       </c>
@@ -7315,7 +7312,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>576</v>
       </c>
@@ -7338,7 +7335,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>578</v>
       </c>
@@ -7361,7 +7358,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>584</v>
       </c>
@@ -7384,7 +7381,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>586</v>
       </c>
@@ -7407,7 +7404,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>588</v>
       </c>
@@ -7432,11 +7429,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7448,22 +7440,22 @@
       <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" customWidth="1"/>
-    <col min="8" max="8" width="128.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="128.33203125" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40" customWidth="1"/>
     <col min="10" max="10" width="98" customWidth="1"/>
-    <col min="15" max="15" width="75.28515625" customWidth="1"/>
+    <col min="15" max="15" width="75.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7495,7 +7487,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7524,7 +7516,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>631</v>
       </c>
@@ -7545,7 +7537,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>271</v>
       </c>
@@ -7566,7 +7558,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>283</v>
       </c>
@@ -7587,7 +7579,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>284</v>
       </c>
@@ -7608,7 +7600,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -7631,7 +7623,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -7651,7 +7643,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -7671,7 +7663,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>210</v>
       </c>
@@ -7691,7 +7683,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -7711,7 +7703,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -7731,7 +7723,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>212</v>
       </c>
@@ -7751,7 +7743,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>213</v>
       </c>
@@ -7771,11 +7763,11 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>279</v>
       </c>
@@ -7796,7 +7788,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -7817,7 +7809,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>267</v>
       </c>
@@ -7838,7 +7830,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>221</v>
       </c>
@@ -7859,7 +7851,7 @@
       </c>
       <c r="I19" s="23"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>222</v>
       </c>
@@ -7879,7 +7871,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>197</v>
       </c>
@@ -7899,7 +7891,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>199</v>
       </c>
@@ -7919,7 +7911,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -7939,7 +7931,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>202</v>
       </c>
@@ -7959,10 +7951,10 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -7986,7 +7978,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>264</v>
       </c>
@@ -8010,7 +8002,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>265</v>
       </c>
@@ -8034,7 +8026,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>130</v>
       </c>
@@ -8055,7 +8047,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>257</v>
       </c>
@@ -8079,7 +8071,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="43" t="s">
         <v>291</v>
       </c>
@@ -8103,7 +8095,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
         <v>292</v>
       </c>
@@ -8127,7 +8119,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -8148,7 +8140,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -8169,7 +8161,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -8190,7 +8182,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -8211,7 +8203,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -8232,7 +8224,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -8250,7 +8242,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -8271,7 +8263,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -8291,7 +8283,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -8311,7 +8303,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -8331,11 +8323,11 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>250</v>
       </c>
@@ -8358,7 +8350,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -8382,10 +8374,10 @@
       </c>
       <c r="J45" s="23"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>595</v>
       </c>
@@ -8407,7 +8399,7 @@
       </c>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>596</v>
       </c>
@@ -8429,7 +8421,7 @@
       </c>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>597</v>
       </c>
@@ -8451,7 +8443,7 @@
       </c>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>598</v>
       </c>
@@ -8473,7 +8465,7 @@
       </c>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>599</v>
       </c>
@@ -8495,7 +8487,7 @@
       </c>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>600</v>
       </c>
@@ -8517,7 +8509,7 @@
       </c>
       <c r="O52" s="2"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>601</v>
       </c>
@@ -8534,7 +8526,7 @@
       </c>
       <c r="O53" s="2"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>602</v>
       </c>
@@ -8551,7 +8543,7 @@
       </c>
       <c r="O54" s="2"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -8568,7 +8560,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -8585,7 +8577,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -8602,7 +8594,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>135</v>
       </c>
@@ -8619,7 +8611,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -8636,7 +8628,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>162</v>
       </c>
@@ -8654,7 +8646,7 @@
       </c>
       <c r="J60" s="23"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>163</v>
       </c>
@@ -8672,7 +8664,7 @@
       </c>
       <c r="J61" s="23"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -8690,12 +8682,12 @@
       </c>
       <c r="J62" s="23"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="43"/>
       <c r="J63" s="23"/>
     </row>
-    <row r="64" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>633</v>
       </c>
@@ -8721,7 +8713,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -8750,7 +8742,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>138</v>
       </c>
@@ -8779,7 +8771,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>139</v>
       </c>
@@ -8808,7 +8800,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -8834,7 +8826,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -8863,7 +8855,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -8892,7 +8884,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>144</v>
       </c>
@@ -8921,7 +8913,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -8947,7 +8939,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>147</v>
       </c>
@@ -8973,7 +8965,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -8999,7 +8991,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -9025,7 +9017,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>165</v>
       </c>
@@ -9051,7 +9043,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>166</v>
       </c>
@@ -9080,7 +9072,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>167</v>
       </c>
@@ -9109,7 +9101,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>168</v>
       </c>
@@ -9138,7 +9130,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -9164,7 +9156,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -9193,7 +9185,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>172</v>
       </c>
@@ -9222,7 +9214,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -9251,7 +9243,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -9277,7 +9269,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>176</v>
       </c>
@@ -9303,7 +9295,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>177</v>
       </c>
@@ -9329,7 +9321,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>178</v>
       </c>
@@ -9355,11 +9347,11 @@
         <v>621</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>299</v>
       </c>
@@ -9385,7 +9377,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>296</v>
       </c>
@@ -9414,7 +9406,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>297</v>
       </c>
@@ -9440,7 +9432,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>298</v>
       </c>
@@ -9466,7 +9458,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>301</v>
       </c>
@@ -9492,7 +9484,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>300</v>
       </c>
@@ -9518,7 +9510,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -9539,7 +9531,7 @@
       </c>
       <c r="J95" s="23"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>174</v>
       </c>
@@ -9560,7 +9552,7 @@
       </c>
       <c r="J96" s="23"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>140</v>
       </c>
@@ -9581,7 +9573,7 @@
       </c>
       <c r="J97" s="23"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>145</v>
       </c>
@@ -9602,11 +9594,11 @@
       </c>
       <c r="J98" s="23"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="J99" s="23"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>412</v>
       </c>
@@ -9629,7 +9621,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>413</v>
       </c>
@@ -9652,7 +9644,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>414</v>
       </c>
@@ -9675,7 +9667,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>409</v>
       </c>
@@ -9704,7 +9696,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>410</v>
       </c>
@@ -9733,7 +9725,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>411</v>
       </c>
@@ -9759,7 +9751,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>415</v>
       </c>
@@ -9782,7 +9774,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>416</v>
       </c>
@@ -9805,7 +9797,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>417</v>
       </c>
@@ -9828,7 +9820,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>418</v>
       </c>
@@ -9857,7 +9849,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>419</v>
       </c>
@@ -9886,7 +9878,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>420</v>
       </c>
@@ -9912,27 +9904,22 @@
         <v>617</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J113" s="49"/>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J114" s="49"/>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J115" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9944,22 +9931,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>